<commit_message>
use iferror for robust error handling
</commit_message>
<xml_diff>
--- a/MIPCel.xlsx
+++ b/MIPCel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cooperterrill/Desktop/MIPCel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2A5ED7-60F5-C345-A521-692FA8A65C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567F1304-A7A4-9C4F-8B38-D355489DAB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19300" xr2:uid="{95E4A03E-3FED-BF42-ACD2-5D2E65B33E92}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <definedName name="_zero">Sheet1!$A$1</definedName>
     <definedName name="ADD">Sheet1!$D$18</definedName>
     <definedName name="ADDI">Sheet1!$M$18</definedName>
-    <definedName name="ALU">Sheet1!$E$15</definedName>
+    <definedName name="ALU">Sheet1!$W$14</definedName>
     <definedName name="AND">Sheet1!$H$18</definedName>
     <definedName name="ANDI">Sheet1!$N$18</definedName>
     <definedName name="BEQ">Sheet1!$R$18</definedName>
@@ -970,8 +970,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:DX201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="132" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="132" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -979,50 +979,52 @@
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" customWidth="1"/>
     <col min="8" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" customWidth="1"/>
+    <col min="20" max="20" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" cm="1">
-        <f t="array" aca="1" ref="A1" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_zero))</f>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_zero)))</f>
+        <v>1680</v>
+      </c>
+      <c r="B1" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_v0)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C1">
+        <f ca="1">IFERROR(IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_v1))),_v1)</f>
         <v>0</v>
       </c>
-      <c r="B1" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_v0))</f>
+      <c r="D1" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_a0)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E1">
+        <f ca="1">IFERROR(IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_a1))),_a1)</f>
         <v>0</v>
       </c>
-      <c r="C1" cm="1">
-        <f t="array" aca="1" ref="C1" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_v1))</f>
-        <v>0</v>
-      </c>
-      <c r="D1" cm="1">
-        <f t="array" aca="1" ref="D1" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_a0))</f>
-        <v>0</v>
-      </c>
-      <c r="E1" cm="1">
-        <f t="array" aca="1" ref="E1" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_a1))</f>
-        <v>0</v>
-      </c>
-      <c r="F1" cm="1">
-        <f t="array" aca="1" ref="F1" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_a2))</f>
-        <v>0</v>
-      </c>
-      <c r="G1" cm="1">
-        <f t="array" aca="1" ref="G1" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_a3))</f>
-        <v>0</v>
-      </c>
-      <c r="H1" cm="1">
-        <f t="array" aca="1" ref="H1" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t0))</f>
-        <v>0</v>
+      <c r="F1" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_a2)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G1" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_a3)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H1" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t0)))</f>
+        <v>#NAME?</v>
       </c>
       <c r="T1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1057,44 +1059,44 @@
       <c r="P2" s="3"/>
       <c r="T2">
         <f ca="1">CLK</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" cm="1">
-        <f t="array" aca="1" ref="A3" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t1))</f>
-        <v>255</v>
-      </c>
-      <c r="B3" cm="1">
-        <f t="array" aca="1" ref="B3" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t2))</f>
-        <v>0</v>
-      </c>
-      <c r="C3" cm="1">
-        <f t="array" aca="1" ref="C3" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t3))</f>
-        <v>0</v>
-      </c>
-      <c r="D3" cm="1">
-        <f t="array" aca="1" ref="D3" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t4))</f>
-        <v>0</v>
-      </c>
-      <c r="E3" cm="1">
-        <f t="array" aca="1" ref="E3" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t5))</f>
-        <v>0</v>
-      </c>
-      <c r="F3" cm="1">
-        <f t="array" aca="1" ref="F3" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t6))</f>
-        <v>0</v>
-      </c>
-      <c r="G3" cm="1">
-        <f t="array" aca="1" ref="G3" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t7))</f>
-        <v>0</v>
-      </c>
-      <c r="H3" cm="1">
-        <f t="array" aca="1" ref="H3" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t8))</f>
-        <v>0</v>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t1)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B3">
+        <f ca="1">IFERROR(IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t2))),_t2)</f>
+        <v>384</v>
+      </c>
+      <c r="C3" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t3)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D3" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t4)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E3" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t5)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F3" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t6)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G3" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t7)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H3" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t8)))</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1128,41 +1130,41 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" cm="1">
-        <f t="array" aca="1" ref="A5" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t9))</f>
-        <v>0</v>
-      </c>
-      <c r="B5" cm="1">
-        <f t="array" aca="1" ref="B5" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s0))</f>
-        <v>0</v>
-      </c>
-      <c r="C5" cm="1">
-        <f t="array" aca="1" ref="C5" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s1))</f>
-        <v>0</v>
-      </c>
-      <c r="D5" cm="1">
-        <f t="array" aca="1" ref="D5" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s2))</f>
-        <v>0</v>
-      </c>
-      <c r="E5" cm="1">
-        <f t="array" aca="1" ref="E5" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s3))</f>
-        <v>0</v>
-      </c>
-      <c r="F5" cm="1">
-        <f t="array" aca="1" ref="F5" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s4))</f>
-        <v>0</v>
-      </c>
-      <c r="G5" cm="1">
-        <f t="array" aca="1" ref="G5" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s5))</f>
-        <v>0</v>
-      </c>
-      <c r="H5" cm="1">
-        <f t="array" aca="1" ref="H5" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s6))</f>
-        <v>0</v>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t9)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B5" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s0)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C5" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s1)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D5" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s2)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E5" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s3)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s4)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G5" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s5)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H5" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s6)))</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -1196,41 +1198,41 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" cm="1">
-        <f t="array" aca="1" ref="A7" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s7))</f>
-        <v>0</v>
-      </c>
-      <c r="B7" cm="1">
-        <f t="array" aca="1" ref="B7" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t8))</f>
-        <v>0</v>
-      </c>
-      <c r="C7" cm="1">
-        <f t="array" aca="1" ref="C7" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t9))</f>
-        <v>0</v>
-      </c>
-      <c r="D7" cm="1">
-        <f t="array" aca="1" ref="D7" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_gp))</f>
-        <v>0</v>
-      </c>
-      <c r="E7" cm="1">
-        <f t="array" aca="1" ref="E7" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_sp))</f>
-        <v>0</v>
-      </c>
-      <c r="F7" cm="1">
-        <f t="array" aca="1" ref="F7" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_fp))</f>
-        <v>0</v>
-      </c>
-      <c r="G7" cm="1">
-        <f t="array" aca="1" ref="G7" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_ra))</f>
-        <v>0</v>
-      </c>
-      <c r="H7" cm="1">
-        <f t="array" aca="1" ref="H7" ca="1">(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_pc))</f>
-        <v>0</v>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_s7)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B7" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t8)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C7" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_t9)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D7" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_gp)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E7" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_sp)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F7" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_fp)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G7" t="e">
+        <f ca="1">IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_ra)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H7">
+        <f ca="1">IFERROR(IF(CLR,0,(IF(REGWRITEADDR=ADDRESS(ROW(),COLUMN()),ALU,_pc))),_pc)</f>
+        <v>1680</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1264,13 +1266,13 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V14" t="s">
         <v>31</v>
       </c>
-      <c r="E15" cm="1">
-        <f t="array" aca="1" ref="E15" ca="1">_xlfn.SWITCH(OP,8,ADDI,12,ANDI,13,ORI,14,XORI,2,J,4,BEQ,5,BNE,34,LW,42,SW, 0, _xlfn.SWITCH(FNCT,32,ADD,34,SUB,24,MULT,26,DIV,36,AND,37,OR,38,XOR,0,SLL,2,SRL))</f>
-        <v>255</v>
+      <c r="W14" cm="1">
+        <f t="array" aca="1" ref="W14" ca="1">IFERROR(_xlfn.SWITCH(OP,8,ADDI,12,ANDI,13,ORI,14,XORI,2,J,4,BEQ,5,BNE,34,LW,42,SW, 0, _xlfn.SWITCH(FNCT,32,ADD,34,SUB,24,MULT,26,DIV,36,AND,37,OR,38,XOR,0,SLL,2,SRL)),ALU)</f>
+        <v>1680</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -1335,11 +1337,11 @@
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D18">
         <f ca="1">RTVAL+RSVAL</f>
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="E18">
         <f ca="1">RSVAL-RTVAL</f>
-        <v>-255</v>
+        <v>-384</v>
       </c>
       <c r="F18">
         <f ca="1">RSVAL*RTVAL</f>
@@ -1355,23 +1357,23 @@
       </c>
       <c r="I18">
         <f ca="1">_xlfn.BITOR(RSVAL,RTVAL)</f>
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="J18">
         <f ca="1">_xlfn.BITXOR(RSVAL,RTVAL)</f>
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="K18">
         <f ca="1">_xlfn.BITLSHIFT(RTVAL,SHMT)</f>
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="L18">
         <f ca="1">_xlfn.BITRSHIFT(RTVAL,SHMT)</f>
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="M18">
         <f ca="1">RSVAL+IMMD</f>
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="N18">
         <f ca="1">_xlfn.BITAND(RSVAL,IMMD)</f>
@@ -1379,31 +1381,31 @@
       </c>
       <c r="O18">
         <f ca="1">_xlfn.BITOR(RSVAL,IMMD)</f>
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="P18">
-        <f ca="1">_xlfn.BITXOR(RSVAL,IMMD)</f>
-        <v>255</v>
+        <f ca="1">IFERROR(_xlfn.BITXOR(RSVAL,IMMD),XORI)</f>
+        <v>384</v>
       </c>
       <c r="Q18">
         <f ca="1">_xlfn.BITOR(_xlfn.BITAND(_pc+4,4026531840),_xlfn.BITLSHIFT(JBITS,2))</f>
-        <v>0</v>
+        <v>1680</v>
       </c>
       <c r="R18">
         <f ca="1">IF(RSVAL=RTVAL,_xlfn.BITLSHIFT(IMMD,2)+_pc+4,_pc+4)</f>
-        <v>4</v>
+        <v>1684</v>
       </c>
       <c r="S18">
         <f ca="1">IF(RSVAL&lt;&gt;RTVAL,_xlfn.BITLSHIFT(IMMD,2)+_pc+4,_pc+4)</f>
-        <v>1024</v>
-      </c>
-      <c r="T18" cm="1">
+        <v>3220</v>
+      </c>
+      <c r="T18" t="e" cm="1">
         <f t="array" aca="1" ref="T18" ca="1">INDIRECT(LWBASEADDR)+IMMD</f>
-        <v>255</v>
+        <v>#NAME?</v>
       </c>
       <c r="U18">
         <f ca="1">RTVAL</f>
-        <v>255</v>
+        <v>384</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1471,7 +1473,7 @@
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <f ca="1">IF(CLR = 1, 0, $A$20 + 1)</f>
-        <v>1570</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
@@ -1480,14 +1482,14 @@
       </c>
       <c r="D22" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDIRECT(RTADDR)</f>
-        <v>255</v>
+        <v>384</v>
       </c>
       <c r="F22" t="s">
         <v>97</v>
       </c>
       <c r="G22" t="str">
         <f>ADDRESS(_xlfn.BITRSHIFT(REGWRITE,3)*2 + 1, 1+_xlfn.BITAND(REGWRITE,7))</f>
-        <v>$A$3</v>
+        <v>$H$7</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
@@ -1501,9 +1503,9 @@
       <c r="F23" t="s">
         <v>66</v>
       </c>
-      <c r="G23" cm="1">
-        <f t="array" ref="G23">IF(RFMT, RD, IF(IFMT,IF(_xlfn.BITRSHIFT(OP,3)=0,pc,RT),pc))</f>
-        <v>8</v>
+      <c r="G23">
+        <f>IF(RFMT, RD, IF(IFMT,IF(_xlfn.BITRSHIFT(OP,3)=0,31,RT),31))</f>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
@@ -1527,8 +1529,8 @@
         <v>23</v>
       </c>
       <c r="D27" t="str">
-        <f>ADDRESS(_xlfn.BITRSHIFT(RT,3)*2 + 1, 1+_xlfn.BITAND(RT,7))</f>
-        <v>$A$3</v>
+        <f ca="1">ADDRESS(_xlfn.BITRSHIFT(RT,3)*2 + 1, 1+_xlfn.BITAND(RT,7))</f>
+        <v>$B$3</v>
       </c>
       <c r="E27" t="s">
         <v>44</v>
@@ -1543,8 +1545,8 @@
         <v>22</v>
       </c>
       <c r="D28" t="str">
-        <f>ADDRESS(_xlfn.BITRSHIFT(RS,3)*2 + 1, 1+_xlfn.BITAND(RS,7))</f>
-        <v>$A$1</v>
+        <f ca="1">ADDRESS(_xlfn.BITRSHIFT(RS,3)*2 + 1, 1+_xlfn.BITAND(RS,7))</f>
+        <v>$E$1</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
@@ -1552,22 +1554,22 @@
         <v>25</v>
       </c>
       <c r="D31">
-        <f ca="1">IF(RFMT, _xlfn.BITAND(INSTR,127),$D$31)</f>
-        <v>32</v>
+        <f xml:space="preserve"> _xlfn.BITAND(INSTR,127)</f>
+        <v>36</v>
       </c>
       <c r="E31" t="s">
         <v>24</v>
       </c>
       <c r="F31">
-        <f>IF(IFMT,_xlfn.BITAND(INSTR,65535),IMMD)</f>
-        <v>255</v>
+        <f ca="1">IF(IFMT,_xlfn.BITAND(INSTR,65535),IMMD)</f>
+        <v>384</v>
       </c>
       <c r="G31" t="s">
         <v>43</v>
       </c>
       <c r="H31">
-        <f ca="1">IF(JFMT,_xlfn.BITAND(INSTR,134217727),JBITS)</f>
-        <v>0</v>
+        <f>IF(JFMT,_xlfn.BITAND(INSTR,134217727),JBITS)</f>
+        <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
@@ -1593,8 +1595,8 @@
         <v>28</v>
       </c>
       <c r="D34">
-        <f>IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,16),31),$D$34)</f>
-        <v>8</v>
+        <f ca="1">IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,16),31),$D$34)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -1602,17 +1604,17 @@
         <v>29</v>
       </c>
       <c r="D35">
-        <f>IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,21),31),$D$35)</f>
-        <v>0</v>
+        <f ca="1">IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,21),31),$D$35)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>537395455</v>
+        <v>134218148</v>
       </c>
       <c r="B36">
         <f>_xlfn.BITRSHIFT($A$36,26)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -1637,11 +1639,11 @@
       </c>
       <c r="E37" t="b">
         <f>AND(NOT(RFMT),NOT(JFMT))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="b">
         <f>OR(OP=2,OP=3,OP=26)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -18512,7 +18514,7 @@
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <f ca="1">IF($A$200 = 1,0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B200" s="2">
         <v>0</v>

</xml_diff>